<commit_message>
next update after deploy; changed some things in the report, cleaned up the app, and fromatted the matrix item
</commit_message>
<xml_diff>
--- a/PRP_QUANT_V2_itemtypes_sheet_16.xlsx
+++ b/PRP_QUANT_V2_itemtypes_sheet_16.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mueller_admin.ZPIDNB21\Documents\Desktop\Rprojects\scripts\prp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mueller_admin.ZPIDNB21\Documents\Desktop\Rprojects\PRP-QUANT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBF113B-CC0A-4D11-A448-F5AB6B7EA28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553943ED-B111-4735-897E-79A4B301B7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="7" xr2:uid="{74259089-353E-4943-B28F-F01CFF5DD15F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{74259089-353E-4943-B28F-F01CFF5DD15F}"/>
   </bookViews>
   <sheets>
     <sheet name="Titlepage" sheetId="1" r:id="rId1"/>
@@ -332,9 +332,6 @@
   </si>
   <si>
     <t>All authors declare that they have no conflicts of interest in the conduct of this study. tab There is a potential conflict of interest.</t>
-  </si>
-  <si>
-    <t>as public use file tab as scientific use file tab on case basis tab via secure data center tab per email request tab none tab not applicable</t>
   </si>
   <si>
     <t>Include the best estimate for how long the project will take from preregistration submission to project completion.</t>
@@ -1253,6 +1250,9 @@
   </si>
   <si>
     <t>This document was created using the Psychological Research Preregistration-Quantitative (aka PRP-QUANT) Template, version 3 (available at https://www.psycharchives.org/). tab The PRP-QUANT Template was originally developed by a task force composed of members of the American Psychological Association (APA), the British Psychological Society (BPS), the German Psychological Society (DGPs), the Center for Open Science (COS), and the Leibniz Institute for Psychology (ZPID). This work is licensed under the CC BY 4.0 license. Thus, you are free to share and adapt the content, given that you attribute the source and indicate if changes were made. tab At the annual meeting of the Society for Psychological Science (SIPS), version 3 was developed by a group of members in a hackathon in Padova, Italy in 2023. tab The implementation as Shiny app was done by ZPID. Find out more about ZPID and our preregistration service PreReg by visiting https://leibniz-psychology.org/ and http://prereg-psych.org/, respectively. tab To receive a timestamp and a citable DOI, submit your preregistration protocol as a PDF to PsychArchives via https://pasa.psycharchives.org/.</t>
+  </si>
+  <si>
+    <t>**as public use file** tab **as scientific use file** tab **on case basis** tab **via secure data center** tab **per email request** tab **none** tab **not applicable**</t>
   </si>
 </sst>
 </file>
@@ -1900,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E096B71-D52A-4541-A0A9-91CC8576266F}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,16 +1958,16 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
         <v>56</v>
       </c>
       <c r="K2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1987,13 +1987,13 @@
         <v>93</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
         <v>57</v>
       </c>
       <c r="K3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2022,13 +2022,13 @@
         <v>94</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J4" t="s">
         <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2054,13 +2054,13 @@
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s">
         <v>58</v>
       </c>
       <c r="K5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2086,16 +2086,16 @@
         <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J6" t="s">
         <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2115,13 +2115,13 @@
         <v>95</v>
       </c>
       <c r="I7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J7" t="s">
         <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2147,13 +2147,13 @@
         <v>92</v>
       </c>
       <c r="I8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2170,16 +2170,16 @@
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" t="s">
         <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2199,13 +2199,13 @@
         <v>93</v>
       </c>
       <c r="I10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J10" t="s">
         <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2231,13 +2231,13 @@
         <v>90</v>
       </c>
       <c r="I11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J11" t="s">
         <v>60</v>
       </c>
       <c r="K11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L11" t="s">
         <v>54</v>
@@ -2257,16 +2257,16 @@
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>96</v>
+        <v>310</v>
       </c>
       <c r="I12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J12" t="s">
         <v>61</v>
       </c>
       <c r="K12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2283,16 +2283,16 @@
         <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J13" t="s">
         <v>61</v>
       </c>
       <c r="K13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2309,13 +2309,13 @@
         <v>20</v>
       </c>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J14" t="s">
         <v>62</v>
       </c>
       <c r="K14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2373,54 +2373,54 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2481,91 +2481,91 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -2574,24 +2574,24 @@
         <v>93</v>
       </c>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -2600,22 +2600,22 @@
         <v>23</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2676,13 +2676,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -2693,24 +2693,24 @@
         <v>93</v>
       </c>
       <c r="I2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -2719,151 +2719,151 @@
         <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -2875,13 +2875,13 @@
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J9" t="s">
         <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2939,134 +2939,134 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3078,13 +3078,13 @@
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J7" t="s">
         <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3142,261 +3142,261 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
@@ -3405,24 +3405,24 @@
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G12" t="s">
         <v>90</v>
       </c>
       <c r="I12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3434,13 +3434,13 @@
         <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3452,7 +3452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E34F2CD-01B9-4150-A4F1-563976AEF5F4}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -3498,45 +3498,45 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K3" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
updated small stuff based on Lisas feedback and saving state before changing how the Word report is created in the downloadHandler
</commit_message>
<xml_diff>
--- a/PRP_QUANT_V2_itemtypes_sheet_16.xlsx
+++ b/PRP_QUANT_V2_itemtypes_sheet_16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mueller_admin.ZPIDNB21\Documents\Desktop\Rprojects\PRP-QUANT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553943ED-B111-4735-897E-79A4B301B7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E707F40F-C3C2-4557-A8ED-DA0D8EC2617C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{74259089-353E-4943-B28F-F01CFF5DD15F}"/>
+    <workbookView xWindow="-26580" yWindow="2460" windowWidth="21600" windowHeight="12645" firstSheet="4" activeTab="7" xr2:uid="{74259089-353E-4943-B28F-F01CFF5DD15F}"/>
   </bookViews>
   <sheets>
     <sheet name="Titlepage" sheetId="1" r:id="rId1"/>
@@ -1249,10 +1249,10 @@
     <t>If you test hypotheses in your study: Specify the statistical model (e.g. t-test, ANOVA, LMM) that will be used to test each of your hypotheses. Give all necessary information about model specification (e.g., variables, interactions, planned contrasts) and follow-up analyses. Include model selection criteria (e.g., fit indices), corrections for multiple testing, and tests for statistical violations, if applicable.</t>
   </si>
   <si>
-    <t>This document was created using the Psychological Research Preregistration-Quantitative (aka PRP-QUANT) Template, version 3 (available at https://www.psycharchives.org/). tab The PRP-QUANT Template was originally developed by a task force composed of members of the American Psychological Association (APA), the British Psychological Society (BPS), the German Psychological Society (DGPs), the Center for Open Science (COS), and the Leibniz Institute for Psychology (ZPID). This work is licensed under the CC BY 4.0 license. Thus, you are free to share and adapt the content, given that you attribute the source and indicate if changes were made. tab At the annual meeting of the Society for Psychological Science (SIPS), version 3 was developed by a group of members in a hackathon in Padova, Italy in 2023. tab The implementation as Shiny app was done by ZPID. Find out more about ZPID and our preregistration service PreReg by visiting https://leibniz-psychology.org/ and http://prereg-psych.org/, respectively. tab To receive a timestamp and a citable DOI, submit your preregistration protocol as a PDF to PsychArchives via https://pasa.psycharchives.org/.</t>
-  </si>
-  <si>
     <t>**as public use file** tab **as scientific use file** tab **on case basis** tab **via secure data center** tab **per email request** tab **none** tab **not applicable**</t>
+  </si>
+  <si>
+    <t>This document was created using the Psychological Research Preregistration-Quantitative (aka PRP-QUANT) Template, version 3 (available at https://www.psycharchives.org/). tab The PRP-QUANT Template was originally developed by a task force composed of members of the American Psychological Association (APA), the British Psychological Society (BPS), the German Psychological Society (DGPs), the Center for Open Science (COS), and the Leibniz Institute for Psychology (ZPID). This work is licensed under the CC BY 4.0 license. Thus, you are free to share and adapt the content, given that you attribute the source and indicate if changes were made. tab At the annual meeting of the Society for Psychological Science (SIPS), version 3 was developed by a group of members in a hackathon in Padova, Italy in 2023. tab The implementation as Shiny app was done by ZPID. Find out more about ZPID and our preregistration service PreReg by visiting https://leibniz-psychology.org/ and http://prereg-psych.org/, respectively. tab To receive a timestamp and a DOI, submit your preregistration protocol as a PDF to PsychArchives via https://pasa.psycharchives.org/.</t>
   </si>
 </sst>
 </file>
@@ -1900,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E096B71-D52A-4541-A0A9-91CC8576266F}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -2257,7 +2257,7 @@
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I12" t="s">
         <v>105</v>
@@ -3452,8 +3452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E34F2CD-01B9-4150-A4F1-563976AEF5F4}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3536,7 +3536,7 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K3" t="s">
         <v>50</v>

</xml_diff>